<commit_message>
llm call sucessful, output getting generated with less accuracy
</commit_message>
<xml_diff>
--- a/data/cases_output_with_pbm.xlsx
+++ b/data/cases_output_with_pbm.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Request:Check user type; must be Customer or Employee.:Educate</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>#PBM:NA:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Data:Investigate data sync issue between Remedy and Service Desk.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>#PBM:NA:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Customization:Error editing questionnaire; check customization settings.:NA</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:NA:See case notes:NA</t>
+          <t>#PBM:DWPC:Permissions:Granted administrator permissions to specified users.:Customization</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Integration:Guide on automating user creation via API for DWP access.:Educate</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Defect:Date format inconsistency; consult R&amp;D for expected behavior.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Request:Investigate request cancellation delay issue.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Workflow:Investigate workflow approval delay and request creation issue.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>#PBM:SRM:NA:See case notes:NA</t>
+          <t>#PBM:SRM:Report:Guide on mapping SRM fields to Helix Dashboard equivalents.:Educate</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:NA:See case notes:NA</t>
+          <t>#PBM:DWPC:Data:Provided guidance on credential encryption/decryption in DWPC.:Educate</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Notification Template:Disabled 'Waiting approval' notification via DB query.:Customization</t>
         </is>
       </c>
     </row>
@@ -756,7 +756,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Configuration:Increased autoclose duration to 1 year post-upgrade.:Customization</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>#PBM:NA:NA:See case notes:NA</t>
+          <t>#PBM:SRM:Workflow:Investigate SR status sync issue with completed WOs.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>#PBM:NA:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Multitenancy:Setup enhanced catalog for sub tenant on production.:Customization</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:NA:See case notes:NA</t>
+          <t>#PBM:DWPC:Log:Investigate logs for deactivation cause.:NA</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>#PBM:NA:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Request:Manually updated request status to completed.:NA</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Broadcast:Broadcast not fully removed; sync issue suspected.:NA</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Configuration:Check reCAPTCHA v3 configuration and adjust settings.:Educate</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>#PBM:DWP:NA:See case notes:NA</t>
+          <t>#PBM:DWP:Customization:Educated on customizing comment display settings.:Educate</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:NA:See case notes:NA</t>
+          <t>#PBM:DWPC:Configuration:Page error when enabling services in chatbot; check configuration settings.:NA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
run.py and app.py working properly
</commit_message>
<xml_diff>
--- a/data/cases_output_with_pbm.xlsx
+++ b/data/cases_output_with_pbm.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Request:Check user type; must be Customer or Employee.:Educate</t>
+          <t>#PBM:DWP:Request:Check user roles and company association for 'On behalf of' requests.:Educate</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Data:Investigate data sync issue between Remedy and Service Desk.:R&amp;D</t>
+          <t>#PBM:DWP:Data:Mismatch in ticket status between user profile and Service Desk.:NA</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Integration:Guide on automating user creation via API for DWP access.:Educate</t>
+          <t>#PBM:DWP:Integration:Guide on automating user access via API.:Educate</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Request:Investigate request cancellation delay issue.:R&amp;D</t>
+          <t>#PBM:DWP:Request:Investigate request cancellation delay in DWP.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Multitenancy:Setup enhanced catalog for sub tenant on production.:Customization</t>
+          <t>#PBM:DWP:Multitenancy:Enhanced catalog setup for sub tenant on production.:Customization</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Broadcast:Broadcast not fully removed; sync issue suspected.:NA</t>
+          <t>#PBM:DWP:Broadcast:Broadcast not removed due to sync issue; needs manual update.:NA</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Customization:Educated on customizing comment display settings.:Educate</t>
+          <t>#PBM:DWP:Customization:Usernames in comments can be customized via settings.:Educate</t>
         </is>
       </c>
     </row>

</xml_diff>